<commit_message>
20XWO8: Excel Practice2 done Practice3 start
</commit_message>
<xml_diff>
--- a/20XWO8 - DATA VISUALIZATION/Practice2/Practice2.xlsx
+++ b/20XWO8 - DATA VISUALIZATION/Practice2/Practice2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\20XWO8 - DATA VISUALIZATION\Practice2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\college8\20XWO8 - DATA VISUALIZATION\Practice2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A1A6DB-FC27-4D8E-90CE-C1C120BAA8C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8620EA77-9580-49B6-8FB4-DC8EBDAF0F61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Exercise 1</t>
   </si>
@@ -191,12 +191,102 @@
   <si>
     <t>TOTAL</t>
   </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>(Urban - City Limits)</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Mumbai (Bombay)</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Dilli (Delhi)</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Korea (South)</t>
+  </si>
+  <si>
+    <t>Sao Paulo</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Munchkins Sales Trends</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Exercise 6</t>
+  </si>
+  <si>
+    <t>Exercise 7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,8 +357,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,8 +404,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -427,11 +532,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -443,15 +557,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,25 +581,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,6 +616,54 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,6 +1379,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1250,6 +1399,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1265,6 +1419,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1280,6 +1439,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1468,6 +1632,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1483,6 +1652,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1498,6 +1672,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1513,6 +1692,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1528,6 +1712,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1543,6 +1732,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1690,6 +1884,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1705,6 +1904,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1720,6 +1924,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1735,6 +1944,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1750,6 +1964,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1765,6 +1984,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-19E3-4033-A4F2-9F21F7C86F30}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2108,6 +2332,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2128,6 +2357,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2148,6 +2382,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2168,6 +2407,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2188,6 +2432,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2208,6 +2457,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2230,6 +2484,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2280,6 +2539,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-7F83-48B9-B9B2-8C1BB323E69A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3558,6 +3822,857 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="9000">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="45000">
+                  <a:srgbClr val="7030A0"/>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+              </a:path>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$97:$A$106</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Crunchie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mars Bar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Yorkie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dairy Crunch</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Cadburys Dairy Milk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Snickers</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hershey Bar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lindt Lindor Bar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>KitKat</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dime Bar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$97:$B$107</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$97:$B$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3523-4E22-ACF9-049396C08146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>France</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="sphere">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$97:$A$106</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Crunchie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mars Bar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Yorkie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dairy Crunch</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Cadburys Dairy Milk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Snickers</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hershey Bar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lindt Lindor Bar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>KitKat</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dime Bar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$97:$C$107</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$97:$C$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3523-4E22-ACF9-049396C08146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1939692815"/>
+        <c:axId val="1981466527"/>
+        <c:axId val="1451172880"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>USA</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:sp3d/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$97:$A$106</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Crunchie</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Mars Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Yorkie</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Dairy Crunch</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Cadburys Dairy Milk</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Snickers</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Hershey Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lindt Lindor Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>KitKat</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Dime Bar</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$D$97:$D$107</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$97:$D$106</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3523-4E22-ACF9-049396C08146}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Germany</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:sp3d/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$97:$A$106</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Crunchie</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Mars Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Yorkie</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Dairy Crunch</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Cadburys Dairy Milk</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Snickers</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Hershey Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lindt Lindor Bar</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>KitKat</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Dime Bar</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$E$97:$E$107</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$97:$E$106</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3523-4E22-ACF9-049396C08146}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1939692815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1981466527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1981466527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1939692815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1451172880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1981466527"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3590,8 +4705,8 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="90"/>
-      <c:rotY val="90"/>
+      <c:rotX val="30"/>
+      <c:rotY val="80"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
@@ -3639,31 +4754,22 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$96</c:f>
+              <c:f>Sheet1!$D$120:$D$121</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>UK</c:v>
+                  <c:v>Population</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(Urban - City Limits)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="9000">
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="45000">
-                  <a:srgbClr val="7030A0"/>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-              </a:path>
-            </a:gradFill>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -3673,209 +4779,85 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$97:$A$107</c:f>
+              <c:f>Sheet1!$B$122:$B$131</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Crunchie</c:v>
+                  <c:v>Shanghai</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Mars Bar</c:v>
+                  <c:v>Mumbai (Bombay)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Yorkie</c:v>
+                  <c:v>Karachi</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Dairy Crunch</c:v>
+                  <c:v>Buenos Aires</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Cadburys Dairy Milk</c:v>
+                  <c:v>Dilli (Delhi)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Snickers</c:v>
+                  <c:v>Manila</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Hershey Bar</c:v>
+                  <c:v>Moscow</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Lindt Lindor Bar</c:v>
+                  <c:v>Seoul</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>KitKat</c:v>
+                  <c:v>Sao Paulo</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Dime Bar</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>TOTAL</c:v>
+                  <c:v>Istanbul</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$97:$B$107</c:f>
+              <c:f>Sheet1!$D$122:$D$131</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>14608512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>12691836</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>11624219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>11574205</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>10927986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>10444527</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>10381222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>10349312</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>10210295</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>9792428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:shape val="cone"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3523-4E22-ACF9-049396C08146}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$96</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>France</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="sphere">
-              <a:fgClr>
-                <a:srgbClr val="FF0000"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$97:$A$107</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>Crunchie</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Mars Bar</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yorkie</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Dairy Crunch</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Cadburys Dairy Milk</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Snickers</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Hershey Bar</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Lindt Lindor Bar</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>KitKat</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Dime Bar</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$97:$C$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3523-4E22-ACF9-049396C08146}"/>
+              <c16:uniqueId val="{00000000-928F-416E-B353-8DFD105E8BB1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3887,292 +4869,80 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="140"/>
+        <c:gapWidth val="0"/>
+        <c:gapDepth val="203"/>
         <c:shape val="box"/>
-        <c:axId val="1939692815"/>
-        <c:axId val="1981466527"/>
+        <c:axId val="1282945312"/>
+        <c:axId val="1308170864"/>
         <c:axId val="0"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$96</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>USA</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                  <a:sp3d/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="11"/>
-                      <c:pt idx="0">
-                        <c:v>Crunchie</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Mars Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Yorkie</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>Dairy Crunch</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>Cadburys Dairy Milk</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Snickers</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Hershey Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Lindt Lindor Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>KitKat</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Dime Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>TOTAL</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$97:$D$107</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="11"/>
-                      <c:pt idx="0">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>38</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-3523-4E22-ACF9-049396C08146}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="3"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$96</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Germany</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent4"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                  <a:sp3d/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$97:$A$107</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="11"/>
-                      <c:pt idx="0">
-                        <c:v>Crunchie</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Mars Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Yorkie</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>Dairy Crunch</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>Cadburys Dairy Milk</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Snickers</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Hershey Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Lindt Lindor Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>KitKat</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Dime Bar</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>TOTAL</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$97:$E$107</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="11"/>
-                      <c:pt idx="0">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-3523-4E22-ACF9-049396C08146}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1939692815"/>
+        <c:axId val="1282945312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1308170864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="10"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1308170864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4203,15 +4973,368 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1981466527"/>
+        <c:crossAx val="1282945312"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Year</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$139:$B$140</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Munchkins Sales Trends</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$141:$A$150</c:f>
+              <c:numCache>
+                <c:formatCode>_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>23800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$141:$B$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0EBC-445C-951E-6836C010DC25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1194115584"/>
+        <c:axId val="1395735776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1194115584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="40000"/>
+          <c:min val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1395735776"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1981466527"/>
+        <c:axId val="1395735776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4221,7 +5344,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4259,9 +5385,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1939692815"/>
+        <c:crossAx val="1194115584"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4271,37 +5397,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4586,6 +5681,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -7236,6 +8411,495 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="296">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7697,6 +9361,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7915,16 +10082,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>16328</xdr:rowOff>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7944,6 +10111,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11204</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>449035</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>55347</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89D33B5A-9989-483D-80BB-B20AEA2499AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16529</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>16529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3984BE8-DD70-46DA-9E00-C6C93044D9FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8215,17 +10454,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S110" sqref="S110"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N137" sqref="N137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8235,11 +10475,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -8322,107 +10562,107 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="8">
         <v>0.17</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="9">
         <v>0.31</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="9">
         <v>0.18</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="10">
         <v>0.2</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="11">
         <v>0.15</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="11">
         <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="10">
         <v>0.04</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="11">
         <v>0.19</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="11">
         <v>0.41</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="10">
         <v>0.34</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="11">
         <v>0.12</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="11">
         <v>0.03</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="10">
         <v>0.17</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="11">
         <v>0.08</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="11">
         <v>0.11</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="10">
         <v>0.08</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="11">
         <v>0.15</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="11">
         <v>0.26</v>
       </c>
     </row>
@@ -8432,88 +10672,88 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="38"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="14">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="14">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="14">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="14">
         <v>12</v>
       </c>
     </row>
@@ -8523,240 +10763,240 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="39"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="21">
+      <c r="A66" s="16">
         <v>1</v>
       </c>
-      <c r="B66" s="21">
+      <c r="B66" s="16">
         <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="21">
+      <c r="A67" s="16">
         <v>2</v>
       </c>
-      <c r="B67" s="21">
+      <c r="B67" s="16">
         <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="21">
+      <c r="A68" s="16">
         <v>3</v>
       </c>
-      <c r="B68" s="21">
+      <c r="B68" s="16">
         <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="21">
+      <c r="A69" s="16">
         <v>4</v>
       </c>
-      <c r="B69" s="21">
+      <c r="B69" s="16">
         <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="21">
+      <c r="A70" s="16">
         <v>5</v>
       </c>
-      <c r="B70" s="21">
+      <c r="B70" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="21">
+      <c r="A71" s="16">
         <v>6</v>
       </c>
-      <c r="B71" s="21">
+      <c r="B71" s="16">
         <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="21">
+      <c r="A72" s="16">
         <v>7</v>
       </c>
-      <c r="B72" s="21">
+      <c r="B72" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="21">
+      <c r="A73" s="16">
         <v>8</v>
       </c>
-      <c r="B73" s="21">
+      <c r="B73" s="16">
         <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="21">
+      <c r="A74" s="16">
         <v>9</v>
       </c>
-      <c r="B74" s="21">
+      <c r="B74" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="21">
+      <c r="A75" s="16">
         <v>10</v>
       </c>
-      <c r="B75" s="21">
+      <c r="B75" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="21">
+      <c r="A76" s="16">
         <v>11</v>
       </c>
-      <c r="B76" s="21">
+      <c r="B76" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="21">
+      <c r="A77" s="16">
         <v>12</v>
       </c>
-      <c r="B77" s="21">
+      <c r="B77" s="16">
         <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="21">
+      <c r="A78" s="16">
         <v>13</v>
       </c>
-      <c r="B78" s="21">
+      <c r="B78" s="16">
         <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="21">
+      <c r="A79" s="16">
         <v>14</v>
       </c>
-      <c r="B79" s="21">
+      <c r="B79" s="16">
         <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="21">
+      <c r="A80" s="16">
         <v>15</v>
       </c>
-      <c r="B80" s="21">
+      <c r="B80" s="16">
         <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="21">
+      <c r="A81" s="16">
         <v>16</v>
       </c>
-      <c r="B81" s="21">
+      <c r="B81" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="21">
+      <c r="A82" s="16">
         <v>17</v>
       </c>
-      <c r="B82" s="21">
+      <c r="B82" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="21">
+      <c r="A83" s="16">
         <v>18</v>
       </c>
-      <c r="B83" s="21">
+      <c r="B83" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="21">
+      <c r="A84" s="16">
         <v>19</v>
       </c>
-      <c r="B84" s="21">
+      <c r="B84" s="16">
         <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="21">
+      <c r="A85" s="16">
         <v>20</v>
       </c>
-      <c r="B85" s="21">
+      <c r="B85" s="16">
         <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="21">
+      <c r="A86" s="16">
         <v>21</v>
       </c>
-      <c r="B86" s="21">
+      <c r="B86" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="21">
+      <c r="A87" s="16">
         <v>22</v>
       </c>
-      <c r="B87" s="21">
+      <c r="B87" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="21">
+      <c r="A88" s="16">
         <v>23</v>
       </c>
-      <c r="B88" s="21">
+      <c r="B88" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="21">
+      <c r="A89" s="16">
         <v>24</v>
       </c>
-      <c r="B89" s="21">
+      <c r="B89" s="16">
         <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="21">
+      <c r="A90" s="16">
         <v>25</v>
       </c>
-      <c r="B90" s="21">
+      <c r="B90" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="21">
+      <c r="A91" s="16">
         <v>26</v>
       </c>
-      <c r="B91" s="21">
+      <c r="B91" s="16">
         <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="21">
+      <c r="A92" s="16">
         <v>27</v>
       </c>
-      <c r="B92" s="21">
+      <c r="B92" s="16">
         <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="21">
+      <c r="A93" s="16">
         <v>28</v>
       </c>
-      <c r="B93" s="21">
+      <c r="B93" s="16">
         <v>165</v>
       </c>
     </row>
@@ -8766,215 +11006,486 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="23" t="s">
+      <c r="A96" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B96" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C96" s="24" t="s">
+      <c r="C96" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D96" s="24" t="s">
+      <c r="D96" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E96" s="24" t="s">
+      <c r="E96" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B97" s="26">
+      <c r="B97" s="20">
         <v>12</v>
       </c>
-      <c r="C97" s="27">
+      <c r="C97" s="21">
         <v>1</v>
       </c>
-      <c r="D97" s="27">
+      <c r="D97" s="21">
         <v>2</v>
       </c>
-      <c r="E97" s="27">
+      <c r="E97" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="25" t="s">
+      <c r="A98" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B98" s="28">
+      <c r="B98" s="22">
         <v>25</v>
       </c>
-      <c r="C98" s="29">
+      <c r="C98" s="23">
         <v>7</v>
       </c>
-      <c r="D98" s="29">
+      <c r="D98" s="23">
         <v>11</v>
       </c>
-      <c r="E98" s="29">
+      <c r="E98" s="23">
         <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="25" t="s">
+      <c r="A99" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B99" s="28">
+      <c r="B99" s="22">
         <v>8</v>
       </c>
-      <c r="C99" s="29">
+      <c r="C99" s="23">
         <v>2</v>
       </c>
-      <c r="D99" s="29">
+      <c r="D99" s="23">
         <v>1</v>
       </c>
-      <c r="E99" s="29">
+      <c r="E99" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B100" s="28">
+      <c r="B100" s="22">
         <v>1</v>
       </c>
-      <c r="C100" s="29">
+      <c r="C100" s="23">
         <v>1</v>
       </c>
-      <c r="D100" s="29">
+      <c r="D100" s="23">
         <v>7</v>
       </c>
-      <c r="E100" s="29">
+      <c r="E100" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="25" t="s">
+      <c r="A101" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B101" s="28">
+      <c r="B101" s="22">
         <v>18</v>
       </c>
-      <c r="C101" s="29">
+      <c r="C101" s="23">
         <v>13</v>
       </c>
-      <c r="D101" s="29">
+      <c r="D101" s="23">
         <v>9</v>
       </c>
-      <c r="E101" s="29">
+      <c r="E101" s="23">
         <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B102" s="28">
+      <c r="B102" s="22">
         <v>6</v>
       </c>
-      <c r="C102" s="29">
+      <c r="C102" s="23">
         <v>1</v>
       </c>
-      <c r="D102" s="29">
+      <c r="D102" s="23">
         <v>11</v>
       </c>
-      <c r="E102" s="29">
+      <c r="E102" s="23">
         <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="25" t="s">
+      <c r="A103" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B103" s="28">
+      <c r="B103" s="22">
         <v>2</v>
       </c>
-      <c r="C103" s="29">
+      <c r="C103" s="23">
         <v>8</v>
       </c>
-      <c r="D103" s="29">
+      <c r="D103" s="23">
         <v>38</v>
       </c>
-      <c r="E103" s="29">
+      <c r="E103" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="25" t="s">
+      <c r="A104" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B104" s="28">
+      <c r="B104" s="22">
         <v>4</v>
       </c>
-      <c r="C104" s="29">
+      <c r="C104" s="23">
         <v>39</v>
       </c>
-      <c r="D104" s="29">
+      <c r="D104" s="23">
         <v>5</v>
       </c>
-      <c r="E104" s="29">
+      <c r="E104" s="23">
         <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="25" t="s">
+      <c r="A105" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B105" s="28">
+      <c r="B105" s="22">
         <v>20</v>
       </c>
-      <c r="C105" s="29">
+      <c r="C105" s="23">
         <v>17</v>
       </c>
-      <c r="D105" s="29">
+      <c r="D105" s="23">
         <v>14</v>
       </c>
-      <c r="E105" s="29">
+      <c r="E105" s="23">
         <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B106" s="28">
+      <c r="B106" s="22">
         <v>4</v>
       </c>
-      <c r="C106" s="29">
+      <c r="C106" s="23">
         <v>11</v>
       </c>
-      <c r="D106" s="29">
+      <c r="D106" s="23">
         <v>2</v>
       </c>
-      <c r="E106" s="29">
+      <c r="E106" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="23" t="s">
+      <c r="A107" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B107" s="30">
+      <c r="B107" s="24">
         <v>100</v>
       </c>
-      <c r="C107" s="30">
+      <c r="C107" s="24">
         <v>100</v>
       </c>
-      <c r="D107" s="30">
+      <c r="D107" s="24">
         <v>100</v>
       </c>
-      <c r="E107" s="30">
+      <c r="E107" s="24">
         <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B120" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C120" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D120" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="26">
+        <v>1</v>
+      </c>
+      <c r="B122" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D122" s="27">
+        <v>14608512</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="26">
+        <v>2</v>
+      </c>
+      <c r="B123" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C123" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D123" s="27">
+        <v>12691836</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="26">
+        <v>3</v>
+      </c>
+      <c r="B124" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C124" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D124" s="27">
+        <v>11624219</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="26">
+        <v>4</v>
+      </c>
+      <c r="B125" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D125" s="27">
+        <v>11574205</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="26">
+        <v>5</v>
+      </c>
+      <c r="B126" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C126" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D126" s="27">
+        <v>10927986</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="26">
+        <v>6</v>
+      </c>
+      <c r="B127" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D127" s="27">
+        <v>10444527</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="26">
+        <v>7</v>
+      </c>
+      <c r="B128" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D128" s="27">
+        <v>10381222</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="26">
+        <v>8</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D129" s="27">
+        <v>10349312</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="26">
+        <v>9</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D130" s="27">
+        <v>10210295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="26">
+        <v>10</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C131" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D131" s="27">
+        <v>9792428</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B139" s="33"/>
+      <c r="C139" s="28"/>
+    </row>
+    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B140" s="30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="32">
+        <v>23800</v>
+      </c>
+      <c r="B141" s="31">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="32">
+        <v>26400</v>
+      </c>
+      <c r="B142" s="31">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="32">
+        <v>23700</v>
+      </c>
+      <c r="B143" s="31">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="32">
+        <v>31900</v>
+      </c>
+      <c r="B144" s="31">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="32">
+        <v>28500</v>
+      </c>
+      <c r="B145" s="31">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="32">
+        <v>32700</v>
+      </c>
+      <c r="B146" s="31">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="32">
+        <v>35700</v>
+      </c>
+      <c r="B147" s="31">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="32">
+        <v>29500</v>
+      </c>
+      <c r="B148" s="31">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="32">
+        <v>37500</v>
+      </c>
+      <c r="B149" s="31">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="32">
+        <v>39700</v>
+      </c>
+      <c r="B150" s="31">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A139:B139"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>